<commit_message>
the last sunday commit
</commit_message>
<xml_diff>
--- a/docs/BugReport.xlsx
+++ b/docs/BugReport.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BUG_01" sheetId="1" r:id="rId1"/>
+    <sheet name="BUG_02" sheetId="2" r:id="rId2"/>
+    <sheet name="BUG_03" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="50">
   <si>
     <t>Category</t>
   </si>
@@ -132,13 +134,62 @@
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>BUG_02</t>
+  </si>
+  <si>
+    <t>Mục lịch sử tìm kiếm ở thanh tìm kiếm không biến mất khi đã xóa hết lịch sử tìm kiếm</t>
+  </si>
+  <si>
+    <t>Mục lịch sử tìm kiếm ở thanh tìm kiếm không biến mất</t>
+  </si>
+  <si>
+    <t>https://www.fahasa.com</t>
+  </si>
+  <si>
+    <t>B1: Truy cập: www.fahasa.com
+B2: Nhấn chọn ô tìm kiếm
+B3: Chọn xóa một mục tìm kiếm
+B4: Chọn xóa tất cả</t>
+  </si>
+  <si>
+    <t>Khi nhấn biểu tượng dấu x tại tên sản phẩm từng tìm thì tên đó sẽ biến mất, các tag sau sẽ dồn về bên trái
+Khi chọn xóa hết tất cả lịch sử tìm kiếm thì mục lịch sử tìm kiếm sẽ biến mất</t>
+  </si>
+  <si>
+    <t>Khi nhấn biểu tượng dấu x tại tên sản phẩm từng tìm thì tên đó sẽ biến mất, các tag sau sẽ dồn về bên trái
+Khi mục lịch sử tìm kiếm vẫn còn hiển thị</t>
+  </si>
+  <si>
+    <t>BUG_03</t>
+  </si>
+  <si>
+    <t>Hiển thị kết quả tìm kiếm sản phẩm bị cắt</t>
+  </si>
+  <si>
+    <t>Khi hiển thị kết quả timf kiếm ở điện thoại 412x914 ở hướng dọc các sản phẩm ở cột thứ 4 bị cắt</t>
+  </si>
+  <si>
+    <t>B1: Truy cập: www.fahasa.com
+B2: Nhấn chọn ô tìm kiếm
+B3: Nhập: 'Conan'
+B4: Chọn nút tìm kiếm
+B5: Chọn sản phẩm "Túi Vải Conan"</t>
+  </si>
+  <si>
+    <t>Không thành phần nào bị che, lấp, sản phẩm hiển thị đầy đủ, rõ ràng
+Thông tin sản phẩm hiển thị rõ ràng, đẩy đủ, hình sản sản phẩm không bị mất hay bị cắt</t>
+  </si>
+  <si>
+    <t>Tại kết quả tìm kiếm sản phẩm, khi hiển thị theo hướng dọc sản phẩm ở cột thứ 4 bị cắt mất</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +212,16 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -195,16 +256,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -214,10 +273,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -270,6 +336,92 @@
         <a:xfrm>
           <a:off x="3394608" y="1315538"/>
           <a:ext cx="5339575" cy="2110324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1790096</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>60476</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6144380</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2103511</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3955144" y="1330476"/>
+          <a:ext cx="4354284" cy="2043035"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1731818</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>25978</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3217925</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>3293509</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3896591" y="1298864"/>
+          <a:ext cx="1486107" cy="3267531"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -570,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="119" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -593,163 +745,163 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="7"/>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>45645</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="7"/>
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="171" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="7"/>
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -765,4 +917,406 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="3" max="3" width="120.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="171" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A17"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="3" max="3" width="82.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="262.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="66" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A17"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>